<commit_message>
database plan updated for project 3
</commit_message>
<xml_diff>
--- a/project03/tavernDB_plan.xlsx
+++ b/project03/tavernDB_plan.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wlgro\Documents\MTwdbc\project02\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wlgro\Documents\MTwdbc\project03\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C05C9B8D-8745-4762-9890-B50BDD6F4186}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29D379F5-5DFA-4F5D-94D1-348F15108405}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0C740F7E-A40E-4004-A829-37DED4AD7C50}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="66">
   <si>
     <t>taverns</t>
   </si>
@@ -105,9 +105,6 @@
     <t>Date: 2/28/19</t>
   </si>
   <si>
-    <t>Version: 1.0</t>
-  </si>
-  <si>
     <t>userInfo</t>
   </si>
   <si>
@@ -199,6 +196,39 @@
   </si>
   <si>
     <t>guestClasses</t>
+  </si>
+  <si>
+    <t>roomRecords</t>
+  </si>
+  <si>
+    <t>room_ID*</t>
+  </si>
+  <si>
+    <t>sale_ID*</t>
+  </si>
+  <si>
+    <t>rooms</t>
+  </si>
+  <si>
+    <t>roomNumber</t>
+  </si>
+  <si>
+    <t>checkOut</t>
+  </si>
+  <si>
+    <t>checkIn</t>
+  </si>
+  <si>
+    <t>pricePerNight</t>
+  </si>
+  <si>
+    <t>roomStatuses</t>
+  </si>
+  <si>
+    <t>roomStatus_ID*</t>
+  </si>
+  <si>
+    <t>Version: 1.2</t>
   </si>
 </sst>
 </file>
@@ -222,7 +252,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -301,8 +331,32 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.499984740745262"/>
+        <bgColor theme="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -362,11 +416,39 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -388,15 +470,30 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -484,8 +581,8 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{E0313658-BE98-44C4-A5EF-E85C335A6F08}" name="Table12" displayName="Table12" ref="K13:K20" totalsRowShown="0">
-  <autoFilter ref="K13:K20" xr:uid="{652B734C-A0CD-419C-B888-F23686DB823B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{E0313658-BE98-44C4-A5EF-E85C335A6F08}" name="Table12" displayName="Table12" ref="E23:E30" totalsRowShown="0">
+  <autoFilter ref="E23:E30" xr:uid="{652B734C-A0CD-419C-B888-F23686DB823B}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{DBA2D4E4-53FE-4E83-8711-5754E4E4E11C}" name="orders"/>
   </tableColumns>
@@ -494,18 +591,8 @@
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{4F2C4954-8A20-4486-BE7E-0C84415CE640}" name="Table13" displayName="Table13" ref="M13:M19" totalsRowShown="0">
-  <autoFilter ref="M13:M19" xr:uid="{57054837-248C-435C-81CC-5C24885158EC}"/>
-  <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{EE19AD34-4EE5-44BD-91A0-2CAA588F520F}" name="sales"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{4CB56E77-DF6D-4104-88AD-577CB2EE4243}" name="Table9" displayName="Table9" ref="O13:O18" totalsRowShown="0">
-  <autoFilter ref="O13:O18" xr:uid="{DCB6CCE4-7913-4438-ABF2-BF1065BDB3C8}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{4CB56E77-DF6D-4104-88AD-577CB2EE4243}" name="Table9" displayName="Table9" ref="I23:I28" totalsRowShown="0">
+  <autoFilter ref="I23:I28" xr:uid="{DCB6CCE4-7913-4438-ABF2-BF1065BDB3C8}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{D29CD843-3E38-4C53-8220-E290B9F7AD62}" name="serviceSupplies"/>
   </tableColumns>
@@ -513,11 +600,21 @@
 </table>
 </file>
 
-<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{6F2EF3DE-AEA3-4A36-9970-D58C091A95ED}" name="Table5" displayName="Table5" ref="G23:G26" totalsRowShown="0">
-  <autoFilter ref="G23:G26" xr:uid="{B79B363E-8874-4BCB-94EA-D070620B9FB0}"/>
+<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{6F2EF3DE-AEA3-4A36-9970-D58C091A95ED}" name="Table5" displayName="Table5" ref="O23:O26" totalsRowShown="0">
+  <autoFilter ref="O23:O26" xr:uid="{B79B363E-8874-4BCB-94EA-D070620B9FB0}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{7AEF54BB-8075-4D4A-81F8-32CBBF8C8686}" name="guestClasses"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{FBF33379-B424-4970-85D6-14BA0FCD22DC}" name="Table14" displayName="Table14" ref="G23:G28" totalsRowShown="0">
+  <autoFilter ref="G23:G28" xr:uid="{06E0073E-5CFC-4FB5-8045-D62054374EB6}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{B4455AE1-752D-423D-B9AE-89F11867C45D}" name="roomRecords"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -554,8 +651,8 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{9FE0EB35-79A4-4DFC-9119-7B9E221EE218}" name="Table7" displayName="Table7" ref="E23:E26" totalsRowShown="0">
-  <autoFilter ref="E23:E26" xr:uid="{88D9DDB3-F95C-48D6-8F90-82D0A9B085DE}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{9FE0EB35-79A4-4DFC-9119-7B9E221EE218}" name="Table7" displayName="Table7" ref="M23:M26" totalsRowShown="0">
+  <autoFilter ref="M23:M26" xr:uid="{88D9DDB3-F95C-48D6-8F90-82D0A9B085DE}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{4104F8A5-14A9-4402-9B3E-0858EDCB6101}" name="userInfo"/>
   </tableColumns>
@@ -564,8 +661,8 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{B424434C-92D3-4766-B20A-FE9BEBA7CC29}" name="Table39" displayName="Table39" ref="E13:E20" totalsRowShown="0" headerRowBorderDxfId="1">
-  <autoFilter ref="E13:E20" xr:uid="{09E8337E-8920-46B5-A10B-CC0EE69AF291}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{B424434C-92D3-4766-B20A-FE9BEBA7CC29}" name="Table39" displayName="Table39" ref="G13:G20" totalsRowShown="0" headerRowBorderDxfId="1">
+  <autoFilter ref="G13:G20" xr:uid="{09E8337E-8920-46B5-A10B-CC0EE69AF291}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{4A750CEF-BB89-4295-84BD-46EDBCA0B20E}" name="locations"/>
   </tableColumns>
@@ -574,8 +671,8 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{90DD2A3B-9B2F-4E7F-AE80-5AC149959B78}" name="Table3" displayName="Table3" ref="G13:G19" totalsRowShown="0" headerRowBorderDxfId="0">
-  <autoFilter ref="G13:G19" xr:uid="{57E399F1-F9D4-4D4C-8469-C8EF0893DB21}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{90DD2A3B-9B2F-4E7F-AE80-5AC149959B78}" name="Table3" displayName="Table3" ref="I13:I19" totalsRowShown="0" headerRowBorderDxfId="0">
+  <autoFilter ref="I13:I19" xr:uid="{57E399F1-F9D4-4D4C-8469-C8EF0893DB21}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{7C79CAA0-5975-4B3A-A81B-E499F733901E}" name="guests"/>
   </tableColumns>
@@ -584,8 +681,8 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{40C79247-19A0-4E0B-84A5-473408D59042}" name="Table10" displayName="Table10" ref="C23:C27" totalsRowShown="0">
-  <autoFilter ref="C23:C27" xr:uid="{9823955D-61C9-4EEB-A512-F5F779D89F01}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{40C79247-19A0-4E0B-84A5-473408D59042}" name="Table10" displayName="Table10" ref="K23:K27" totalsRowShown="0">
+  <autoFilter ref="K23:K27" xr:uid="{9823955D-61C9-4EEB-A512-F5F779D89F01}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{5CD34190-B481-4F09-B449-551A4F609BD5}" name="serviceStatuses"/>
   </tableColumns>
@@ -594,8 +691,8 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{C8A11E63-AC69-4A73-A659-95A28A41EB5D}" name="Table11" displayName="Table11" ref="I13:I19" totalsRowShown="0">
-  <autoFilter ref="I13:I19" xr:uid="{071116D3-29E3-47D1-AA51-D708F7ADB922}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{C8A11E63-AC69-4A73-A659-95A28A41EB5D}" name="Table11" displayName="Table11" ref="C23:C29" totalsRowShown="0">
+  <autoFilter ref="C23:C29" xr:uid="{071116D3-29E3-47D1-AA51-D708F7ADB922}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{9377DE04-38AE-4703-9465-C1D34F281DD3}" name="inventory"/>
   </tableColumns>
@@ -900,10 +997,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8ED40847-C0F9-4BC0-A326-1C1410336474}">
-  <dimension ref="A1:O27"/>
+  <dimension ref="A1:O30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -912,8 +1009,8 @@
     <col min="3" max="3" width="16.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.109375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="16.109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -940,7 +1037,7 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -957,16 +1054,16 @@
         <v>3</v>
       </c>
       <c r="I7" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="K7" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="K7" s="16" t="s">
+      <c r="M7" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="M7" s="17" t="s">
-        <v>30</v>
-      </c>
       <c r="O7" s="20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
@@ -1030,239 +1127,291 @@
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A12" s="21" t="s">
-        <v>47</v>
+      <c r="A12" s="27" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="21"/>
-      <c r="C13" s="24" t="s">
-        <v>53</v>
-      </c>
-      <c r="E13" s="7" t="s">
+      <c r="A13" s="27"/>
+      <c r="C13" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="E13" s="39" t="s">
+        <v>63</v>
+      </c>
+      <c r="G13" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="G13" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="I13" t="s">
-        <v>31</v>
-      </c>
-      <c r="K13" t="s">
+      <c r="I13" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="K13" s="40" t="s">
+        <v>58</v>
+      </c>
+      <c r="M13" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="M13" t="s">
-        <v>33</v>
-      </c>
-      <c r="O13" t="s">
-        <v>45</v>
-      </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A14" s="21"/>
-      <c r="C14" s="23" t="s">
-        <v>2</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G14" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="I14" t="s">
-        <v>2</v>
-      </c>
-      <c r="K14" t="s">
-        <v>2</v>
-      </c>
-      <c r="M14" t="s">
-        <v>2</v>
-      </c>
-      <c r="O14" s="5" t="s">
-        <v>13</v>
+      <c r="A14" s="27"/>
+      <c r="C14" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="E14" s="37" t="s">
+        <v>2</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="K14" s="41" t="s">
+        <v>2</v>
+      </c>
+      <c r="M14" s="34" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A15" s="21"/>
+      <c r="A15" s="27"/>
       <c r="C15" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="G15" t="s">
         <v>8</v>
       </c>
-      <c r="G15" t="s">
+      <c r="I15" t="s">
         <v>1</v>
       </c>
-      <c r="I15" s="5" t="s">
+      <c r="K15" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="K15" s="5" t="s">
+      <c r="M15" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="M15" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="O15" s="9" t="s">
-        <v>35</v>
-      </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A16" s="21"/>
-      <c r="E16" t="s">
+      <c r="A16" s="27"/>
+      <c r="G16" t="s">
         <v>9</v>
       </c>
-      <c r="G16" t="s">
+      <c r="I16" t="s">
+        <v>33</v>
+      </c>
+      <c r="K16" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="M16" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="I16" s="8" t="s">
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A17" s="27"/>
+      <c r="G17" t="s">
+        <v>10</v>
+      </c>
+      <c r="I17" t="s">
+        <v>47</v>
+      </c>
+      <c r="K17" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="M17" s="32" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="27"/>
+      <c r="C18" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="G18" t="s">
+        <v>11</v>
+      </c>
+      <c r="I18" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="K18" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="M18" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="K16" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="M16" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="O16" s="8" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A17" s="21"/>
-      <c r="E17" t="s">
-        <v>10</v>
-      </c>
-      <c r="G17" t="s">
-        <v>48</v>
-      </c>
-      <c r="I17" t="s">
-        <v>38</v>
-      </c>
-      <c r="K17" t="s">
-        <v>38</v>
-      </c>
-      <c r="M17" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="O17" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="21"/>
-      <c r="C18" s="26" t="s">
-        <v>50</v>
-      </c>
-      <c r="E18" t="s">
-        <v>11</v>
-      </c>
-      <c r="G18" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="I18" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="K18" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="M18" t="s">
-        <v>38</v>
-      </c>
-      <c r="O18" s="18" t="s">
-        <v>46</v>
-      </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A19" s="21"/>
-      <c r="C19" s="25" t="s">
-        <v>2</v>
-      </c>
-      <c r="E19" t="s">
+      <c r="A19" s="27"/>
+      <c r="C19" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="G19" t="s">
         <v>12</v>
       </c>
-      <c r="G19" t="s">
-        <v>54</v>
-      </c>
       <c r="I19" t="s">
-        <v>40</v>
-      </c>
-      <c r="K19" t="s">
-        <v>41</v>
-      </c>
-      <c r="M19" t="s">
-        <v>40</v>
+        <v>53</v>
+      </c>
+      <c r="K19" s="11"/>
+      <c r="M19" s="29" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A20" s="21"/>
+      <c r="A20" s="27"/>
       <c r="C20" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="G20" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K20" t="s">
-        <v>40</v>
-      </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A21" s="21"/>
+      <c r="A21" s="27"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A22" s="21"/>
+      <c r="A22" s="27"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A23" s="21"/>
+      <c r="A23" s="27"/>
       <c r="C23" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="E23" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="G23" t="s">
         <v>55</v>
       </c>
+      <c r="I23" t="s">
+        <v>44</v>
+      </c>
+      <c r="K23" t="s">
+        <v>43</v>
+      </c>
+      <c r="M23" t="s">
+        <v>24</v>
+      </c>
+      <c r="O23" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A24" s="21"/>
-      <c r="C24" s="5" t="s">
+      <c r="A24" s="27"/>
+      <c r="C24" t="s">
+        <v>2</v>
+      </c>
+      <c r="E24" t="s">
+        <v>2</v>
+      </c>
+      <c r="G24" t="s">
+        <v>2</v>
+      </c>
+      <c r="I24" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E24" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G24" s="6" t="s">
+      <c r="K24" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="M24" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="O24" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A25" s="27"/>
+      <c r="C25" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G25" s="42" t="s">
+        <v>56</v>
+      </c>
+      <c r="I25" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="K25" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="M25" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="O25" s="26" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A26" s="27"/>
+      <c r="C26" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E26" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="G26" s="35" t="s">
+        <v>57</v>
+      </c>
+      <c r="I26" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K26" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A25" s="21"/>
-      <c r="C25" s="9" t="s">
+      <c r="M26" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="O26" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A27" s="27"/>
+      <c r="C27" t="s">
+        <v>37</v>
+      </c>
+      <c r="E27" t="s">
+        <v>37</v>
+      </c>
+      <c r="G27" t="s">
+        <v>61</v>
+      </c>
+      <c r="I27" t="s">
+        <v>37</v>
+      </c>
+      <c r="K27" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="E25" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G25" s="27" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A26" s="21"/>
-      <c r="C26" t="s">
-        <v>43</v>
-      </c>
-      <c r="E26" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G26" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A27" s="21"/>
-      <c r="C27" s="10" t="s">
-        <v>36</v>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="C28" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="E28" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="G28" t="s">
+        <v>60</v>
+      </c>
+      <c r="I28" s="18" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="C29" t="s">
+        <v>39</v>
+      </c>
+      <c r="E29" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="E30" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>